<commit_message>
Changed contest and question form layout.
</commit_message>
<xml_diff>
--- a/wwwroot/Odpovede.xlsx
+++ b/wwwroot/Odpovede.xlsx
@@ -7,15 +7,14 @@
   </bookViews>
   <sheets>
     <sheet name="Skušobná súťaž" sheetId="1" r:id="rId3"/>
-    <sheet name="Dalsia" sheetId="2" r:id="rId4"/>
-    <sheet name="Este jedna" sheetId="3" r:id="rId5"/>
-    <sheet name="ererte" sheetId="4" r:id="rId6"/>
+    <sheet name="Este jedna" sheetId="2" r:id="rId4"/>
+    <sheet name="ererte" sheetId="3" r:id="rId5"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="22">
   <si>
     <t xml:space="preserve">1. Logo prehliadača</t>
   </si>
@@ -32,64 +31,55 @@
     <t xml:space="preserve">Úspešnosť (v %)</t>
   </si>
   <si>
-    <t xml:space="preserve">guest4@frivia.sk</t>
+    <t xml:space="preserve">admin@frivia.sk</t>
   </si>
   <si>
     <t xml:space="preserve">Áno</t>
   </si>
   <si>
+    <t xml:space="preserve">1. gdfgdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2. asdasd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3. hrhr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. asdasd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2. gdfgdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4. Súčet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5. Logo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6. sad</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7. asdasdasd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8. Obrazok</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9. asd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10. dds</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11. ds</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12. Logo prehliadača</t>
+  </si>
+  <si>
     <t xml:space="preserve">Nie</t>
-  </si>
-  <si>
-    <t xml:space="preserve">admin@frivia.sk</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1. gdfgdf</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2. hrhr</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3. asdasd</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2. asdasd</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3. hrhr</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1. asdasd</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2. gdfgdf</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4. Súčet</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5. Logo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6. sad</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7. asdasdasd</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8. Obrazok</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9. asd</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10. dds</t>
-  </si>
-  <si>
-    <t xml:space="preserve">11. ds</t>
-  </si>
-  <si>
-    <t xml:space="preserve">12. Logo prehliadača</t>
   </si>
 </sst>
 </file>
@@ -168,36 +158,16 @@
         <v>6</v>
       </c>
       <c r="D3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G3">
-        <v>66.67</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F4">
-        <v>3</v>
-      </c>
-      <c r="G4">
         <v>100</v>
       </c>
     </row>
-    <row r="5"/>
+    <row r="4"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -214,13 +184,13 @@
     <row r="1">
       <c r="A1"/>
       <c r="B1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" t="s">
         <v>9</v>
-      </c>
-      <c r="C1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D1" t="s">
-        <v>11</v>
       </c>
       <c r="F1" t="s">
         <v>3</v>
@@ -246,72 +216,40 @@
     <row r="1">
       <c r="A1"/>
       <c r="B1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" t="s">
         <v>9</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>12</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>13</v>
       </c>
-      <c r="F1" t="s">
-        <v>3</v>
-      </c>
       <c r="G1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3"/>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView showRuler="1" showOutlineSymbols="1" defaultGridColor="1" colorId="64" zoomScale="100" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1"/>
-      <c r="B1" t="s">
         <v>14</v>
       </c>
-      <c r="C1" t="s">
+      <c r="H1" t="s">
         <v>15</v>
       </c>
-      <c r="D1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="I1" t="s">
         <v>16</v>
       </c>
-      <c r="F1" t="s">
+      <c r="J1" t="s">
         <v>17</v>
       </c>
-      <c r="G1" t="s">
+      <c r="K1" t="s">
         <v>18</v>
       </c>
-      <c r="H1" t="s">
+      <c r="L1" t="s">
         <v>19</v>
       </c>
-      <c r="I1" t="s">
+      <c r="M1" t="s">
         <v>20</v>
-      </c>
-      <c r="J1" t="s">
-        <v>21</v>
-      </c>
-      <c r="K1" t="s">
-        <v>22</v>
-      </c>
-      <c r="L1" t="s">
-        <v>23</v>
-      </c>
-      <c r="M1" t="s">
-        <v>24</v>
       </c>
       <c r="O1" t="s">
         <v>3</v>
@@ -322,10 +260,10 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="C3" t="s">
         <v>6</v>
@@ -337,28 +275,28 @@
         <v>6</v>
       </c>
       <c r="F3" t="s">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="G3" t="s">
         <v>6</v>
       </c>
       <c r="H3" t="s">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="I3" t="s">
         <v>6</v>
       </c>
       <c r="J3" t="s">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="K3" t="s">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="L3" t="s">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="M3" t="s">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="O3">
         <v>5</v>

</xml_diff>

<commit_message>
Added enviroment variable for sql server, fixed unnecessary call on table update, added user account deletion for administrator
</commit_message>
<xml_diff>
--- a/wwwroot/Odpovede.xlsx
+++ b/wwwroot/Odpovede.xlsx
@@ -9,20 +9,24 @@
     <sheet name="Skušobná súťaž" sheetId="1" r:id="rId3"/>
     <sheet name="Este jedna" sheetId="2" r:id="rId4"/>
     <sheet name="ererte" sheetId="3" r:id="rId5"/>
+    <sheet name="Testík" sheetId="4" r:id="rId6"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="22">
-  <si>
-    <t xml:space="preserve">1. Logo prehliadača</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2. Logo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3. Súčet</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="23">
+  <si>
+    <t xml:space="preserve">1. hrhr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2. sad</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3. gdfgdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4. Súčet</t>
   </si>
   <si>
     <t xml:space="preserve">Počet správnych odpovedí</t>
@@ -31,55 +35,55 @@
     <t xml:space="preserve">Úspešnosť (v %)</t>
   </si>
   <si>
+    <t xml:space="preserve">1. gdfgdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2. asdasd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3. hrhr</t>
+  </si>
+  <si>
     <t xml:space="preserve">admin@frivia.sk</t>
   </si>
   <si>
+    <t xml:space="preserve">Nie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nedokončil</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. asdasd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2. gdfgdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5. Logo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6. sad</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7. asdasdasd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8. Obrazok</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9. asd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10. dds</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11. ds</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12. Logo prehliadača</t>
+  </si>
+  <si>
     <t xml:space="preserve">Áno</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1. gdfgdf</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2. asdasd</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3. hrhr</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1. asdasd</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2. gdfgdf</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4. Súčet</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5. Logo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6. sad</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7. asdasdasd</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8. Obrazok</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9. asd</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10. dds</t>
-  </si>
-  <si>
-    <t xml:space="preserve">11. ds</t>
-  </si>
-  <si>
-    <t xml:space="preserve">12. Logo prehliadača</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nie</t>
   </si>
 </sst>
 </file>
@@ -140,34 +144,17 @@
       <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
       <c r="G1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" t="s">
-        <v>6</v>
-      </c>
-      <c r="F3">
-        <v>3</v>
-      </c>
-      <c r="G3">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="4"/>
+      <c r="H1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -184,22 +171,35 @@
     <row r="1">
       <c r="A1"/>
       <c r="B1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" t="s">
         <v>7</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>8</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
         <v>9</v>
       </c>
-      <c r="F1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3"/>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3"/>
+      <c r="D3"/>
+      <c r="F3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -216,87 +216,87 @@
     <row r="1">
       <c r="A1"/>
       <c r="B1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E1" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="F1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="I1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="K1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="L1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="O1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="P1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="D3" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="E3" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="F3" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="G3" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="H3" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="I3" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="J3" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="K3" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="L3" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="M3" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="O3">
         <v>5</v>
@@ -309,4 +309,30 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView showRuler="1" showOutlineSymbols="1" defaultGridColor="1" colorId="64" zoomScale="100" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1"/>
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Otočené poradie v tabuľkách (najnovšie vždy hore).
</commit_message>
<xml_diff>
--- a/wwwroot/Odpovede.xlsx
+++ b/wwwroot/Odpovede.xlsx
@@ -8,12 +8,13 @@
   <sheets>
     <sheet name="Testovacia súťaž" sheetId="1" r:id="rId3"/>
     <sheet name="Ukončená súťaž" sheetId="2" r:id="rId4"/>
+    <sheet name="asdas" sheetId="3" r:id="rId5"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="14">
   <si>
     <t xml:space="preserve"/>
   </si>
@@ -52,6 +53,9 @@
   </si>
   <si>
     <t xml:space="preserve">5. Katedry FRI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Výročie FRI</t>
   </si>
 </sst>
 </file>
@@ -197,4 +201,46 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView showRuler="1" showOutlineSymbols="1" defaultGridColor="1" colorId="64" zoomScale="100" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>